<commit_message>
software fixes, added ANthropic
</commit_message>
<xml_diff>
--- a/TheSoftware/TestResults.xlsx
+++ b/TheSoftware/TestResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geoff/Documents/MyDocuments/Research/Systems/ShZZaM/TheSoftware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC167BB7-701C-964E-897F-23182ADF95F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFCB1E6-EBC4-644C-AB11-55CF37229024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37220" yWindow="620" windowWidth="33660" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,16 +203,16 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -432,8 +432,8 @@
   </sheetPr>
   <dimension ref="A1:R822"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17282,12 +17282,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:K1 I2 I3:K822">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>"I1:I988"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L822">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"BAD"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>